<commit_message>
resolving products and suppliers ids
</commit_message>
<xml_diff>
--- a/exports/incidents_report.xlsx
+++ b/exports/incidents_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>NumRef</t>
   </si>
@@ -46,7 +46,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>02254942</t>
+    <t>03250001</t>
   </si>
   <si>
     <t>COUPURE ELECTRIQUE</t>
@@ -67,13 +67,10 @@
     <t>Admin User</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>CLOTURE</t>
-  </si>
-  <si>
-    <t>02254941</t>
+    <t>dfgdf</t>
+  </si>
+  <si>
+    <t>EN ATTENTE</t>
   </si>
 </sst>
 </file>
@@ -451,7 +448,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -503,7 +500,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="1">
-        <v>45716.729421724536</v>
+        <v>45720.35496090278</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -527,38 +524,6 @@
         <v>18</v>
       </c>
       <c r="K2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45715.651471307865</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added maintenance awaiting validation
</commit_message>
<xml_diff>
--- a/exports/incidents_report.xlsx
+++ b/exports/incidents_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>NumRef</t>
   </si>
@@ -19,6 +19,12 @@
     <t>Date de creation</t>
   </si>
   <si>
+    <t>Date de cloture</t>
+  </si>
+  <si>
+    <t>Durée de résolution</t>
+  </si>
+  <si>
     <t>Type d'incident</t>
   </si>
   <si>
@@ -37,6 +43,9 @@
     <t>Utilisateur</t>
   </si>
   <si>
+    <t>Cloturé par</t>
+  </si>
+  <si>
     <t>description</t>
   </si>
   <si>
@@ -49,6 +58,9 @@
     <t>03250001</t>
   </si>
   <si>
+    <t>175 Heure(s)</t>
+  </si>
+  <si>
     <t>COUPURE ELECTRIQUE</t>
   </si>
   <si>
@@ -67,10 +79,34 @@
     <t>Admin User</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>dfgdf</t>
   </si>
   <si>
-    <t>EN ATTENTE</t>
+    <t>EN MAINTENANCE</t>
+  </si>
+  <si>
+    <t>02254432</t>
+  </si>
+  <si>
+    <t>-482990 Heure(s)</t>
+  </si>
+  <si>
+    <t>GROUPE ELECTROGENE</t>
+  </si>
+  <si>
+    <t>P02</t>
+  </si>
+  <si>
+    <t>FOTSO TSOBGNY FRANCK JOEL</t>
+  </si>
+  <si>
+    <t>On a eu coupure d'électricité sur notre pont</t>
+  </si>
+  <si>
+    <t>CLOTURE</t>
   </si>
 </sst>
 </file>
@@ -448,19 +484,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:N3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="4" width="50" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="50" customWidth="1"/>
-    <col min="10" max="11" width="20" customWidth="1"/>
+    <col min="2" max="3" width="20" customWidth="1"/>
+    <col min="4" max="6" width="50" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="11" width="20" customWidth="1"/>
+    <col min="12" max="12" width="50" customWidth="1"/>
+    <col min="13" max="14" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,37 +530,90 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1">
         <v>45720.35496090278</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
+      <c r="C2" s="1">
+        <v>45727.67790376158</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45693.61901905092</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Handle error messages, incident
</commit_message>
<xml_diff>
--- a/exports/incidents_report.xlsx
+++ b/exports/incidents_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
   <si>
     <t>NumRef</t>
   </si>
@@ -55,58 +55,109 @@
     <t>Status</t>
   </si>
   <si>
+    <t>03250004</t>
+  </si>
+  <si>
+    <t>3 Heure(s)</t>
+  </si>
+  <si>
+    <t>COUPURE ELECTRIQUE</t>
+  </si>
+  <si>
+    <t>L'AXE LOURD ÉTAIT BLOQUE A CAUSE DE LA CAN, CAR DES JOUEURS SORTAIENT POUR LES ENTRAINEMENTS.</t>
+  </si>
+  <si>
+    <t>AIRE DE PESEES</t>
+  </si>
+  <si>
+    <t>SALLE DE CONFERENCE ROOM</t>
+  </si>
+  <si>
+    <t>Shift(14-22)</t>
+  </si>
+  <si>
+    <t>Admin User</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>EN MAINTENANCE</t>
+  </si>
+  <si>
+    <t>03250007</t>
+  </si>
+  <si>
+    <t>19 Heure(s)</t>
+  </si>
+  <si>
+    <t>CAMION EN PANNE DANS LA ZONE DE PRE-PESEE</t>
+  </si>
+  <si>
+    <t>CLOTURE</t>
+  </si>
+  <si>
     <t>03250001</t>
   </si>
   <si>
     <t>175 Heure(s)</t>
   </si>
   <si>
-    <t>COUPURE ELECTRIQUE</t>
-  </si>
-  <si>
-    <t>L'AXE LOURD ÉTAIT BLOQUE A CAUSE DE LA CAN, CAR DES JOUEURS SORTAIENT POUR LES ENTRAINEMENTS.</t>
-  </si>
-  <si>
-    <t>AIRE DE PESEES</t>
-  </si>
-  <si>
     <t>SALLE D'ATTENTE NIVEAU 1</t>
   </si>
   <si>
-    <t>Shift(14-22)</t>
-  </si>
-  <si>
-    <t>Admin User</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>dfgdf</t>
   </si>
   <si>
-    <t>EN MAINTENANCE</t>
-  </si>
-  <si>
-    <t>02254432</t>
+    <t>03250002</t>
+  </si>
+  <si>
+    <t>-483874 Heure(s)</t>
+  </si>
+  <si>
+    <t>Shift(6-14)</t>
+  </si>
+  <si>
+    <t>03250008</t>
+  </si>
+  <si>
+    <t>-483970 Heure(s)</t>
+  </si>
+  <si>
+    <t>RAS</t>
+  </si>
+  <si>
+    <t>02250034</t>
   </si>
   <si>
     <t>-482990 Heure(s)</t>
   </si>
   <si>
-    <t>GROUPE ELECTROGENE</t>
-  </si>
-  <si>
-    <t>P02</t>
-  </si>
-  <si>
-    <t>FOTSO TSOBGNY FRANCK JOEL</t>
-  </si>
-  <si>
-    <t>On a eu coupure d'électricité sur notre pont</t>
-  </si>
-  <si>
-    <t>CLOTURE</t>
+    <t>ENGORGEMENT</t>
+  </si>
+  <si>
+    <t>EMBOUTEILLAGE</t>
+  </si>
+  <si>
+    <t>P03</t>
+  </si>
+  <si>
+    <t>MBAH SONIA</t>
+  </si>
+  <si>
+    <t>Les opérations ont été interrompu au P03 de 13h20-14h05. nous avons eu un embouteillage sur l'axe de l'UDEAC prenant le corridor MESAPRESSE jusqu'au carrefour PARC A BOIS passant par le P18 e</t>
+  </si>
+  <si>
+    <t>03250003</t>
+  </si>
+  <si>
+    <t>-483949 Heure(s)</t>
+  </si>
+  <si>
+    <t>vbnfb</t>
   </si>
 </sst>
 </file>
@@ -484,7 +535,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -545,10 +596,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="1">
-        <v>45720.35496090278</v>
+        <v>45733.571440011576</v>
       </c>
       <c r="C2" s="1">
-        <v>45727.67790376158</v>
+        <v>45733.71721711806</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -586,34 +637,230 @@
         <v>25</v>
       </c>
       <c r="B3" s="1">
-        <v>45693.61901905092</v>
+        <v>45733.625245891206</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45734.4447191088</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K3" t="s">
         <v>22</v>
       </c>
       <c r="L3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45720.35496090278</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45727.67790376158</v>
+      </c>
+      <c r="D4" t="s">
         <v>30</v>
       </c>
-      <c r="N3" t="s">
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
         <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45730.43815700231</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45734.437908148146</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45693.61758100694</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45733.551579293984</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
export by date incident, off-bridges, maintenance
</commit_message>
<xml_diff>
--- a/exports/incidents_report.xlsx
+++ b/exports/incidents_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="42">
   <si>
     <t>NumRef</t>
   </si>
@@ -55,109 +55,88 @@
     <t>Status</t>
   </si>
   <si>
-    <t>03250004</t>
-  </si>
-  <si>
-    <t>3 Heure(s)</t>
+    <t>03250016</t>
+  </si>
+  <si>
+    <t>-483992 Heure(s)</t>
   </si>
   <si>
     <t>COUPURE ELECTRIQUE</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t>AIRE DE PESEES</t>
+  </si>
+  <si>
+    <t>SALLE D'ATTENTE NIVEAU 1</t>
+  </si>
+  <si>
+    <t>Shift(22-6)</t>
+  </si>
+  <si>
+    <t>Admin User</t>
+  </si>
+  <si>
+    <t>CLOTURE</t>
+  </si>
+  <si>
+    <t>03250015</t>
+  </si>
+  <si>
+    <t>CAMION EN PANNE DANS LA ZONE DE PRE-PESEE</t>
+  </si>
+  <si>
+    <t>GROUPE ELECTROGENE</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>Shift(6-14)</t>
+  </si>
+  <si>
+    <t>03250020</t>
+  </si>
+  <si>
+    <t>-483993 Heure(s)</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>EN ATTENTE</t>
+  </si>
+  <si>
+    <t>03250014</t>
+  </si>
+  <si>
+    <t>0 Heure(s)</t>
+  </si>
+  <si>
+    <t>SALLE DE CONFERENCE ROOM</t>
+  </si>
+  <si>
+    <t>03250017</t>
+  </si>
+  <si>
     <t>L'AXE LOURD ÉTAIT BLOQUE A CAUSE DE LA CAN, CAR DES JOUEURS SORTAIENT POUR LES ENTRAINEMENTS.</t>
   </si>
   <si>
-    <t>AIRE DE PESEES</t>
-  </si>
-  <si>
-    <t>SALLE DE CONFERENCE ROOM</t>
-  </si>
-  <si>
-    <t>Shift(14-22)</t>
-  </si>
-  <si>
-    <t>Admin User</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t/>
+    <t>03250019</t>
+  </si>
+  <si>
+    <t>P02</t>
   </si>
   <si>
     <t>EN MAINTENANCE</t>
   </si>
   <si>
-    <t>03250007</t>
-  </si>
-  <si>
-    <t>19 Heure(s)</t>
-  </si>
-  <si>
-    <t>CAMION EN PANNE DANS LA ZONE DE PRE-PESEE</t>
-  </si>
-  <si>
-    <t>CLOTURE</t>
-  </si>
-  <si>
-    <t>03250001</t>
-  </si>
-  <si>
-    <t>175 Heure(s)</t>
-  </si>
-  <si>
-    <t>SALLE D'ATTENTE NIVEAU 1</t>
-  </si>
-  <si>
-    <t>dfgdf</t>
-  </si>
-  <si>
-    <t>03250002</t>
-  </si>
-  <si>
-    <t>-483874 Heure(s)</t>
-  </si>
-  <si>
-    <t>Shift(6-14)</t>
-  </si>
-  <si>
-    <t>03250008</t>
-  </si>
-  <si>
-    <t>-483970 Heure(s)</t>
-  </si>
-  <si>
-    <t>RAS</t>
-  </si>
-  <si>
-    <t>02250034</t>
-  </si>
-  <si>
-    <t>-482990 Heure(s)</t>
-  </si>
-  <si>
-    <t>ENGORGEMENT</t>
-  </si>
-  <si>
-    <t>EMBOUTEILLAGE</t>
-  </si>
-  <si>
-    <t>P03</t>
-  </si>
-  <si>
-    <t>MBAH SONIA</t>
-  </si>
-  <si>
-    <t>Les opérations ont été interrompu au P03 de 13h20-14h05. nous avons eu un embouteillage sur l'axe de l'UDEAC prenant le corridor MESAPRESSE jusqu'au carrefour PARC A BOIS passant par le P18 e</t>
-  </si>
-  <si>
-    <t>03250003</t>
-  </si>
-  <si>
-    <t>-483949 Heure(s)</t>
-  </si>
-  <si>
-    <t>vbnfb</t>
+    <t>03250018</t>
+  </si>
+  <si>
+    <t>INDICATEUR DE POIDS</t>
   </si>
 </sst>
 </file>
@@ -596,10 +575,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="1">
-        <v>45733.571440011576</v>
-      </c>
-      <c r="C2" s="1">
-        <v>45733.71721711806</v>
+        <v>45735.36063092593</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -623,71 +599,65 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" t="s">
         <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45735.34356770833</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="1">
-        <v>45733.625245891206</v>
-      </c>
-      <c r="C3" s="1">
-        <v>45734.4447191088</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="H3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" t="s">
+      <c r="I3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
       <c r="J3" t="s">
         <v>21</v>
       </c>
       <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
         <v>22</v>
-      </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45735.39461263889</v>
+      </c>
+      <c r="D4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="1">
-        <v>45720.35496090278</v>
-      </c>
-      <c r="C4" s="1">
-        <v>45727.67790376158</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -696,36 +666,39 @@
         <v>18</v>
       </c>
       <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" t="s">
         <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45735.210193900464</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45735.21204090278</v>
+      </c>
+      <c r="D5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="1">
-        <v>45730.43815700231</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -734,133 +707,139 @@
         <v>18</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="J5" t="s">
         <v>21</v>
       </c>
       <c r="K5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" t="s">
         <v>22</v>
-      </c>
-      <c r="L5" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45735.3651837963</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
         <v>36</v>
-      </c>
-      <c r="B6" s="1">
-        <v>45734.437908148146</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
       </c>
       <c r="G6" t="s">
         <v>18</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="J6" t="s">
         <v>21</v>
       </c>
       <c r="K6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" t="s">
         <v>22</v>
-      </c>
-      <c r="L6" t="s">
-        <v>38</v>
-      </c>
-      <c r="N6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1">
-        <v>45693.61758100694</v>
+        <v>45735.38652141204</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
         <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
       </c>
       <c r="J7" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="K7" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="L7" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="N7" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B8" s="1">
-        <v>45733.551579293984</v>
+        <v>45735.37092025463</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45735.37163083334</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" t="s">
         <v>27</v>
       </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" t="s">
-        <v>20</v>
-      </c>
       <c r="J8" t="s">
         <v>21</v>
       </c>
       <c r="K8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" t="s">
         <v>22</v>
-      </c>
-      <c r="L8" t="s">
-        <v>48</v>
-      </c>
-      <c r="N8" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added suivi, movement, equipment details
</commit_message>
<xml_diff>
--- a/exports/incidents_report.xlsx
+++ b/exports/incidents_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>NumRef</t>
   </si>
@@ -58,37 +58,61 @@
     <t>Status</t>
   </si>
   <si>
-    <t>04250006</t>
-  </si>
-  <si>
-    <t>7386</t>
-  </si>
-  <si>
-    <t>Type  incident 1</t>
+    <t>06250003</t>
+  </si>
+  <si>
+    <t>N/C</t>
+  </si>
+  <si>
+    <t>Type d'incident 1</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>P19</t>
+  </si>
+  <si>
+    <t>Shift(14-22)</t>
+  </si>
+  <si>
+    <t>Admin User</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>This incident happened due to negligence of the Guerit chef</t>
+  </si>
+  <si>
+    <t>EN MAINTENANCE</t>
+  </si>
+  <si>
+    <t>06250004</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t>Cause incident 1</t>
   </si>
   <si>
-    <t>Ordinateur</t>
-  </si>
-  <si>
-    <t>SALLE DE CONFERENCE ROOM</t>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>NOELLE JEANNE</t>
+  </si>
+  <si>
+    <t>CLOTURE</t>
+  </si>
+  <si>
+    <t>06250001</t>
+  </si>
+  <si>
+    <t>SALLE D'ATTENTE NIVEAU 1</t>
   </si>
   <si>
     <t>Shift(6-14)</t>
-  </si>
-  <si>
-    <t>Admin User</t>
-  </si>
-  <si>
-    <t>2LM</t>
-  </si>
-  <si>
-    <t>klkk</t>
-  </si>
-  <si>
-    <t>CLOTURE</t>
   </si>
 </sst>
 </file>
@@ -482,7 +506,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -546,10 +570,7 @@
         <v>15</v>
       </c>
       <c r="B2" s="2">
-        <v>45771.52749412037</v>
-      </c>
-      <c r="C2" s="2">
-        <v>45776.65680375</v>
+        <v>45819.41148925926</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -560,29 +581,105 @@
       <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>23</v>
       </c>
       <c r="L2" t="s">
         <v>22</v>
       </c>
       <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" t="s">
         <v>24</v>
       </c>
-      <c r="O2" t="s">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>25</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45820.635023090275</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45820.63515135417</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="2">
+        <v>45818.687470613426</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>